<commit_message>
Fixes bug with unmakeMove on AI.stop
</commit_message>
<xml_diff>
--- a/public/ELO Analysis.xlsx
+++ b/public/ELO Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HD/+Node/orobasUI/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00D3685-E5BE-9441-90A3-0C89EF9AE51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFAE764-E93B-C94C-8012-618A420C1E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" xr2:uid="{926F71CF-ED74-EB49-BF4D-0E84ABDC1A78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>LMR</t>
   </si>
@@ -174,13 +174,19 @@
   </si>
   <si>
     <t>Null Window Factor</t>
+  </si>
+  <si>
+    <t>Moves Count Pruning</t>
+  </si>
+  <si>
+    <t>Not fully tested</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,13 +194,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -209,8 +228,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,38 +546,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A865B7B-CB03-CD4F-8C3F-2271F1AAE130}">
-  <dimension ref="B1:G44"/>
+  <dimension ref="B1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="2:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -564,11 +589,11 @@
         <v>400</v>
       </c>
       <c r="D2">
-        <f>C2-$G$1</f>
+        <f>C2-$H$1</f>
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>46</v>
       </c>
@@ -576,11 +601,11 @@
         <v>341</v>
       </c>
       <c r="D3">
-        <f>C3-$G$1</f>
+        <f>C3-$H$1</f>
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -588,11 +613,11 @@
         <v>251</v>
       </c>
       <c r="D4">
-        <f>C4-$G$1</f>
+        <f>C4-$H$1</f>
         <v>240</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>39</v>
       </c>
@@ -600,11 +625,11 @@
         <v>140</v>
       </c>
       <c r="D5">
-        <f>C5-$G$1</f>
+        <f>C5-$H$1</f>
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -612,11 +637,11 @@
         <v>118</v>
       </c>
       <c r="D6">
-        <f>C6-$G$1</f>
+        <f>C6-$H$1</f>
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -624,11 +649,11 @@
         <v>118</v>
       </c>
       <c r="D7">
-        <f>C7-$G$1</f>
+        <f>C7-$H$1</f>
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -636,11 +661,11 @@
         <v>117</v>
       </c>
       <c r="D8">
-        <f>C8-$G$1</f>
+        <f>C8-$H$1</f>
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -648,433 +673,448 @@
         <v>116</v>
       </c>
       <c r="D9">
-        <f>C9-$G$1</f>
+        <f>C9-$H$1</f>
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1">
+        <v>97</v>
+      </c>
+      <c r="D10" s="1">
+        <f>C10-$H$1</f>
+        <v>86</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>84</v>
       </c>
-      <c r="D10">
-        <f>C10-$G$1</f>
+      <c r="D11">
+        <f>C11-$H$1</f>
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>81</v>
       </c>
-      <c r="D11">
-        <f>C11-$G$1</f>
+      <c r="D12">
+        <f>C12-$H$1</f>
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>71</v>
       </c>
-      <c r="D12">
-        <f>C12-$G$1</f>
+      <c r="D13">
+        <f>C13-$H$1</f>
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>67</v>
       </c>
-      <c r="D13">
-        <f>C13-$G$1</f>
+      <c r="D14">
+        <f>C14-$H$1</f>
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>55</v>
       </c>
-      <c r="D14">
-        <f>C14-$G$1</f>
+      <c r="D15">
+        <f>C15-$H$1</f>
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>46</v>
       </c>
-      <c r="D15">
-        <f>C15-$G$1</f>
+      <c r="D16">
+        <f>C16-$H$1</f>
         <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16">
-        <v>45</v>
-      </c>
-      <c r="D16">
-        <f>C16-$G$1</f>
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C17">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17">
-        <f>C17-$G$1</f>
-        <v>32</v>
+        <f>C17-$H$1</f>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="C18">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D18">
-        <f>C18-$G$1</f>
-        <v>28</v>
+        <f>C18-$H$1</f>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <v>39</v>
+      </c>
+      <c r="D19">
+        <f>C19-$H$1</f>
         <v>28</v>
-      </c>
-      <c r="C19">
-        <v>37</v>
-      </c>
-      <c r="D19">
-        <f>C19-$G$1</f>
-        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>37</v>
       </c>
       <c r="D20">
-        <f>C20-$G$1</f>
+        <f>C20-$H$1</f>
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C21">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D21">
-        <f>C21-$G$1</f>
-        <v>22</v>
+        <f>C21-$H$1</f>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C22">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D22">
-        <f>C22-$G$1</f>
-        <v>15</v>
+        <f>C22-$H$1</f>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C23">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D23">
-        <f>C23-$G$1</f>
-        <v>13</v>
+        <f>C23-$H$1</f>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D24">
-        <f>C24-$G$1</f>
-        <v>9</v>
+        <f>C24-$H$1</f>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D25">
-        <f>C25-$G$1</f>
-        <v>8</v>
+        <f>C25-$H$1</f>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C26">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D26">
-        <f>C26-$G$1</f>
-        <v>5</v>
+        <f>C26-$H$1</f>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C27">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D27">
-        <f>C27-$G$1</f>
-        <v>3</v>
+        <f>C27-$H$1</f>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <f>C28-$G$1</f>
-        <v>2</v>
+        <f>C28-$H$1</f>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D29">
-        <f>C29-$G$1</f>
-        <v>-3</v>
+        <f>C29-$H$1</f>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D30">
-        <f>C30-$G$1</f>
-        <v>-11</v>
+        <f>C30-$H$1</f>
+        <v>-3</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <f>C31-$G$1</f>
+        <f>C31-$H$1</f>
         <v>-11</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <f>C32-$G$1</f>
+        <f>C32-$H$1</f>
         <v>-11</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <f>C33-$G$1</f>
+        <f>C33-$H$1</f>
         <v>-11</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <f>C34-$G$1</f>
+        <f>C34-$H$1</f>
         <v>-11</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <f>C35-$G$1</f>
+        <f>C35-$H$1</f>
         <v>-11</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C36">
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <f>C36-$G$1</f>
-        <v>-18</v>
+        <f>C36-$H$1</f>
+        <v>-11</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C37">
-        <v>-10</v>
+        <v>-7</v>
       </c>
       <c r="D37">
-        <f>C37-$G$1</f>
-        <v>-21</v>
+        <f>C37-$H$1</f>
+        <v>-18</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>-10</v>
       </c>
       <c r="D38">
-        <f>C38-$G$1</f>
+        <f>C38-$H$1</f>
         <v>-21</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C39">
-        <v>-27</v>
+        <v>-10</v>
       </c>
       <c r="D39">
-        <f>C39-$G$1</f>
-        <v>-38</v>
+        <f>C39-$H$1</f>
+        <v>-21</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C40">
-        <v>-45</v>
+        <v>-27</v>
       </c>
       <c r="D40">
-        <f>C40-$G$1</f>
-        <v>-56</v>
+        <f>C40-$H$1</f>
+        <v>-38</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C41">
-        <v>-47</v>
+        <v>-45</v>
       </c>
       <c r="D41">
-        <f>C41-$G$1</f>
-        <v>-58</v>
+        <f>C41-$H$1</f>
+        <v>-56</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C42">
-        <v>-49</v>
+        <v>-47</v>
       </c>
       <c r="D42">
-        <f>C42-$G$1</f>
-        <v>-60</v>
+        <f>C42-$H$1</f>
+        <v>-58</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="C43">
-        <v>-50</v>
+        <v>-49</v>
       </c>
       <c r="D43">
-        <f>C43-$G$1</f>
-        <v>-61</v>
+        <f>C43-$H$1</f>
+        <v>-60</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>-50</v>
+      </c>
+      <c r="D44">
+        <f>C44-$H$1</f>
+        <v>-61</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>34</v>
       </c>
-      <c r="C44">
+      <c r="C45">
         <v>-58</v>
       </c>
-      <c r="D44">
-        <f>C44-$G$1</f>
+      <c r="D45">
+        <f>C45-$H$1</f>
         <v>-69</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D44">
-    <sortCondition descending="1" ref="C38:C44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:H45">
+    <sortCondition descending="1" ref="C33:C45"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>